<commit_message>
Fixed author, publisher, warehouse, book upload
</commit_message>
<xml_diff>
--- a/book_rental/management/commands/uploads/inventory_upload.xlsx
+++ b/book_rental/management/commands/uploads/inventory_upload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Code</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>W-000001</t>
+  </si>
+  <si>
+    <t>B-000024</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>Sohel1</t>
+  </si>
+  <si>
+    <t>Hajipara</t>
+  </si>
+  <si>
+    <t>Hajipara 2</t>
   </si>
 </sst>
 </file>
@@ -162,6 +180,35 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>